<commit_message>
Fix barcode import and tests
</commit_message>
<xml_diff>
--- a/spec/etc/valid_barcodes.xlsx
+++ b/spec/etc/valid_barcodes.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t xml:space="preserve">Barcode</t>
   </si>
@@ -29,6 +29,9 @@
   </si>
   <si>
     <t xml:space="preserve">00000093</t>
+  </si>
+  <si>
+    <t xml:space="preserve">314</t>
   </si>
 </sst>
 </file>
@@ -134,17 +137,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:3"/>
+  <dimension ref="1:4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="8.97767857142857"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="8.15178571428571"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="1" width="9.6875"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="8.85714285714286"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="8.03125"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="1" width="9.56696428571429"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3231,6 +3234,11 @@
       <c r="AMI3" s="0"/>
       <c r="AMJ3" s="0"/>
     </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>